<commit_message>
DDA PM BBP TLOS CIF
</commit_message>
<xml_diff>
--- a/src/test/input/used/PM/MVP3 scope for TF_LC_B4-018_PM.xlsx
+++ b/src/test/input/used/PM/MVP3 scope for TF_LC_B4-018_PM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tata\CTBC Trade Finance\Letter of Credit\LC\Document for MVP4 FSD\LC\B4-018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tata\CTBC Trade Finance\Letter of Credit\LC\Document for MVP4 FSD\PM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9931438-0CB0-4862-A03F-651F456981FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C30A8B-3562-4F00-9756-BFE11049A758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="2" xr2:uid="{FD512113-F5B0-4DB7-82FF-ABFE321860E8}"/>
   </bookViews>
@@ -529,9 +529,6 @@
     <t>Create Export Letter Of Credit Parameter</t>
   </si>
   <si>
-    <t>POST /product/{product-ref}/export-letter-of-credit-parameter</t>
-  </si>
-  <si>
     <t>Modify Export Letter Of Credit Parameter</t>
   </si>
   <si>
@@ -568,31 +565,34 @@
     <t>Get Export Doc Collection Parameter</t>
   </si>
   <si>
-    <t>PUT /product/{product-ref}/export-doc-collection-parameter</t>
-  </si>
-  <si>
-    <t>GET /product/{product-ref}/export-doc-collection-parameter</t>
-  </si>
-  <si>
-    <t>POST /product/{product-ref}/export-doc-collection-parameter</t>
+    <t>POST /v2/product/{product-ref}/export-letter-of-credit-parameter</t>
+  </si>
+  <si>
+    <t>POST /v2/product/{product-ref}/export-doc-collection-parameter</t>
+  </si>
+  <si>
+    <t>PUT /v2/product/{product-ref}/export-doc-collection-parameter</t>
+  </si>
+  <si>
+    <t>GET /v2/product/{product-ref}/export-doc-collection-parameter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -654,7 +654,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -686,7 +686,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -712,7 +712,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -723,7 +723,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Aptos Narrow"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -744,6 +744,13 @@
       <color theme="1"/>
       <name val="Tw Cen MT"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="15">
@@ -1328,6 +1335,9 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1345,9 +1355,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1689,7 +1696,7 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="43.42578125" customWidth="1"/>
@@ -1723,7 +1730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75">
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -2018,6 +2025,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2030,7 +2038,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
@@ -2214,7 +2222,7 @@
       <c r="E8" s="20"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2225,7 +2233,7 @@
       <c r="F9" s="13"/>
       <c r="H9" s="16"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2275,7 +2283,7 @@
       <c r="E14" s="20"/>
       <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2286,7 +2294,7 @@
       <c r="F15" s="13"/>
       <c r="H15" s="16"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75">
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2386,7 +2394,7 @@
       <c r="E25" s="20"/>
       <c r="F25" s="13"/>
     </row>
-    <row r="26" spans="1:8" ht="15.75">
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2467,7 +2475,7 @@
       <c r="E33" s="20"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:8" ht="15.75">
+    <row r="34" spans="1:8">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2478,7 +2486,7 @@
       <c r="F34" s="6"/>
       <c r="H34" s="16"/>
     </row>
-    <row r="35" spans="1:8" ht="15.75">
+    <row r="35" spans="1:8">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2489,7 +2497,7 @@
       <c r="F35" s="13"/>
       <c r="H35" s="16"/>
     </row>
-    <row r="36" spans="1:8" ht="15.75">
+    <row r="36" spans="1:8">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2499,7 +2507,7 @@
       <c r="E36" s="33"/>
       <c r="F36" s="13"/>
     </row>
-    <row r="37" spans="1:8" ht="15.75">
+    <row r="37" spans="1:8">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2540,7 +2548,7 @@
       <c r="E40" s="20"/>
       <c r="F40" s="34"/>
     </row>
-    <row r="41" spans="1:8" ht="15.75">
+    <row r="41" spans="1:8">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2550,7 +2558,7 @@
       <c r="E41" s="20"/>
       <c r="F41" s="34"/>
     </row>
-    <row r="42" spans="1:8" ht="15.75">
+    <row r="42" spans="1:8">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2591,7 +2599,7 @@
       <c r="E45" s="20"/>
       <c r="F45" s="34"/>
     </row>
-    <row r="46" spans="1:8" ht="15.75">
+    <row r="46" spans="1:8">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2642,7 +2650,7 @@
       <c r="E50" s="20"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:8" ht="15.75">
+    <row r="51" spans="1:8">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2693,7 +2701,7 @@
       <c r="E55" s="20"/>
       <c r="F55" s="6"/>
     </row>
-    <row r="56" spans="1:8" ht="15.75">
+    <row r="56" spans="1:8">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2711,6 +2719,7 @@
       <c r="B58" s="41"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2719,11 +2728,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75299A52-B02C-4760-8957-A84410B5A1E8}">
   <dimension ref="A1:P278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17:P31"/>
+    <sheetView tabSelected="1" topLeftCell="H19" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="74" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="74" bestFit="1" customWidth="1"/>
@@ -2793,7 +2802,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="30">
+    <row r="2" spans="1:16">
       <c r="A2" s="74" t="s">
         <v>121</v>
       </c>
@@ -2817,7 +2826,7 @@
         <v>twct_EOD_Tracer</v>
       </c>
       <c r="H2" s="75" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I2" s="74" t="s">
         <v>91</v>
@@ -2833,7 +2842,7 @@
         <v>75</v>
       </c>
       <c r="M2" s="74" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="N2" s="75" t="str">
         <f>C2</f>
@@ -2847,7 +2856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="30">
+    <row r="3" spans="1:16">
       <c r="A3" s="74" t="s">
         <v>121</v>
       </c>
@@ -2871,10 +2880,10 @@
         <v>twct_Number_of_Tracers</v>
       </c>
       <c r="H3" s="75" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I3" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J3" s="76" t="s">
         <v>124</v>
@@ -2885,7 +2894,7 @@
       </c>
       <c r="L3" s="77"/>
       <c r="M3" s="74" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="N3" s="75" t="str">
         <f t="shared" ref="N3:N6" si="3">C3</f>
@@ -2899,7 +2908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="30">
+    <row r="4" spans="1:16">
       <c r="A4" s="74" t="s">
         <v>121</v>
       </c>
@@ -2923,10 +2932,10 @@
         <v>twct_Frequency</v>
       </c>
       <c r="H4" s="75" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I4" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J4" s="76" t="s">
         <v>124</v>
@@ -2937,7 +2946,7 @@
       </c>
       <c r="L4" s="77"/>
       <c r="M4" s="74" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="N4" s="75" t="str">
         <f t="shared" si="3"/>
@@ -2951,7 +2960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="30">
+    <row r="5" spans="1:16">
       <c r="A5" s="74" t="s">
         <v>121</v>
       </c>
@@ -2975,10 +2984,10 @@
         <v>twct_Payment_Grace_Days</v>
       </c>
       <c r="H5" s="75" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I5" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J5" s="76" t="s">
         <v>124</v>
@@ -2989,7 +2998,7 @@
       </c>
       <c r="L5" s="77"/>
       <c r="M5" s="74" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="N5" s="75" t="str">
         <f t="shared" si="3"/>
@@ -3003,7 +3012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="30">
+    <row r="6" spans="1:16">
       <c r="A6" s="74" t="s">
         <v>121</v>
       </c>
@@ -3027,10 +3036,10 @@
         <v>twct_Acceptance_Grace_days</v>
       </c>
       <c r="H6" s="75" t="s">
+        <v>133</v>
+      </c>
+      <c r="I6" s="74" t="s">
         <v>134</v>
-      </c>
-      <c r="I6" s="74" t="s">
-        <v>135</v>
       </c>
       <c r="J6" s="76" t="s">
         <v>124</v>
@@ -3041,7 +3050,7 @@
       </c>
       <c r="L6" s="77"/>
       <c r="M6" s="74" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="N6" s="75" t="str">
         <f t="shared" si="3"/>
@@ -3055,7 +3064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="30">
+    <row r="7" spans="1:16">
       <c r="A7" s="74" t="s">
         <v>121</v>
       </c>
@@ -3063,7 +3072,7 @@
         <v>92</v>
       </c>
       <c r="C7" s="106" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D7" s="75" t="s">
         <v>125</v>
@@ -3079,7 +3088,7 @@
         <v>twct_EOD_Tracer</v>
       </c>
       <c r="H7" s="75" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I7" s="74" t="s">
         <v>91</v>
@@ -3095,7 +3104,7 @@
         <v>75</v>
       </c>
       <c r="M7" s="74" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="N7" s="75" t="str">
         <f>C7</f>
@@ -3109,7 +3118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="30">
+    <row r="8" spans="1:16">
       <c r="A8" s="74" t="s">
         <v>121</v>
       </c>
@@ -3117,7 +3126,7 @@
         <v>92</v>
       </c>
       <c r="C8" s="106" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D8" s="75" t="s">
         <v>125</v>
@@ -3133,10 +3142,10 @@
         <v>twct_Number_of_Tracers</v>
       </c>
       <c r="H8" s="75" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I8" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J8" s="76" t="s">
         <v>124</v>
@@ -3147,7 +3156,7 @@
       </c>
       <c r="L8" s="77"/>
       <c r="M8" s="74" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="N8" s="75" t="str">
         <f t="shared" ref="N8:N11" si="7">C8</f>
@@ -3161,7 +3170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="30">
+    <row r="9" spans="1:16">
       <c r="A9" s="74" t="s">
         <v>121</v>
       </c>
@@ -3169,7 +3178,7 @@
         <v>92</v>
       </c>
       <c r="C9" s="106" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D9" s="75" t="s">
         <v>125</v>
@@ -3185,10 +3194,10 @@
         <v>twct_Frequency</v>
       </c>
       <c r="H9" s="75" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I9" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J9" s="76" t="s">
         <v>124</v>
@@ -3199,7 +3208,7 @@
       </c>
       <c r="L9" s="77"/>
       <c r="M9" s="74" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="N9" s="75" t="str">
         <f t="shared" si="7"/>
@@ -3213,7 +3222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="30">
+    <row r="10" spans="1:16">
       <c r="A10" s="74" t="s">
         <v>121</v>
       </c>
@@ -3221,7 +3230,7 @@
         <v>92</v>
       </c>
       <c r="C10" s="106" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D10" s="75" t="s">
         <v>125</v>
@@ -3237,10 +3246,10 @@
         <v>twct_Payment_Grace_Days</v>
       </c>
       <c r="H10" s="75" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I10" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J10" s="76" t="s">
         <v>124</v>
@@ -3251,7 +3260,7 @@
       </c>
       <c r="L10" s="77"/>
       <c r="M10" s="74" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="N10" s="75" t="str">
         <f t="shared" si="7"/>
@@ -3265,7 +3274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="30">
+    <row r="11" spans="1:16">
       <c r="A11" s="74" t="s">
         <v>121</v>
       </c>
@@ -3273,7 +3282,7 @@
         <v>92</v>
       </c>
       <c r="C11" s="106" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D11" s="75" t="s">
         <v>125</v>
@@ -3289,10 +3298,10 @@
         <v>twct_Acceptance_Grace_days</v>
       </c>
       <c r="H11" s="75" t="s">
+        <v>133</v>
+      </c>
+      <c r="I11" s="74" t="s">
         <v>134</v>
-      </c>
-      <c r="I11" s="74" t="s">
-        <v>135</v>
       </c>
       <c r="J11" s="76" t="s">
         <v>124</v>
@@ -3303,7 +3312,7 @@
       </c>
       <c r="L11" s="77"/>
       <c r="M11" s="74" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="N11" s="75" t="str">
         <f t="shared" si="7"/>
@@ -3317,7 +3326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="30">
+    <row r="12" spans="1:16">
       <c r="A12" s="74" t="s">
         <v>121</v>
       </c>
@@ -3325,7 +3334,7 @@
         <v>92</v>
       </c>
       <c r="C12" s="106" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D12" s="75" t="s">
         <v>125</v>
@@ -3341,7 +3350,7 @@
         <v>twct_EOD_Tracer</v>
       </c>
       <c r="H12" s="75" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I12" s="74" t="s">
         <v>91</v>
@@ -3357,7 +3366,7 @@
         <v>75</v>
       </c>
       <c r="M12" s="74" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="N12" s="75" t="str">
         <f>C12</f>
@@ -3371,7 +3380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="30">
+    <row r="13" spans="1:16">
       <c r="A13" s="74" t="s">
         <v>121</v>
       </c>
@@ -3379,7 +3388,7 @@
         <v>92</v>
       </c>
       <c r="C13" s="106" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D13" s="75" t="s">
         <v>125</v>
@@ -3395,10 +3404,10 @@
         <v>twct_Number_of_Tracers</v>
       </c>
       <c r="H13" s="75" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I13" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J13" s="76" t="s">
         <v>124</v>
@@ -3409,7 +3418,7 @@
       </c>
       <c r="L13" s="77"/>
       <c r="M13" s="74" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="N13" s="75" t="str">
         <f t="shared" ref="N13:N16" si="10">C13</f>
@@ -3423,7 +3432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="30">
+    <row r="14" spans="1:16">
       <c r="A14" s="74" t="s">
         <v>121</v>
       </c>
@@ -3431,7 +3440,7 @@
         <v>92</v>
       </c>
       <c r="C14" s="106" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D14" s="75" t="s">
         <v>125</v>
@@ -3447,10 +3456,10 @@
         <v>twct_Frequency</v>
       </c>
       <c r="H14" s="75" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I14" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J14" s="76" t="s">
         <v>124</v>
@@ -3461,7 +3470,7 @@
       </c>
       <c r="L14" s="77"/>
       <c r="M14" s="74" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="N14" s="75" t="str">
         <f t="shared" si="10"/>
@@ -3475,7 +3484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="30">
+    <row r="15" spans="1:16">
       <c r="A15" s="74" t="s">
         <v>121</v>
       </c>
@@ -3483,7 +3492,7 @@
         <v>92</v>
       </c>
       <c r="C15" s="106" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D15" s="75" t="s">
         <v>125</v>
@@ -3499,10 +3508,10 @@
         <v>twct_Payment_Grace_Days</v>
       </c>
       <c r="H15" s="75" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I15" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J15" s="76" t="s">
         <v>124</v>
@@ -3513,7 +3522,7 @@
       </c>
       <c r="L15" s="77"/>
       <c r="M15" s="74" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="N15" s="75" t="str">
         <f t="shared" si="10"/>
@@ -3527,7 +3536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="30">
+    <row r="16" spans="1:16">
       <c r="A16" s="74" t="s">
         <v>121</v>
       </c>
@@ -3535,7 +3544,7 @@
         <v>92</v>
       </c>
       <c r="C16" s="106" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D16" s="75" t="s">
         <v>125</v>
@@ -3551,10 +3560,10 @@
         <v>twct_Acceptance_Grace_days</v>
       </c>
       <c r="H16" s="75" t="s">
+        <v>133</v>
+      </c>
+      <c r="I16" s="74" t="s">
         <v>134</v>
-      </c>
-      <c r="I16" s="74" t="s">
-        <v>135</v>
       </c>
       <c r="J16" s="76" t="s">
         <v>124</v>
@@ -3565,7 +3574,7 @@
       </c>
       <c r="L16" s="77"/>
       <c r="M16" s="74" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="N16" s="75" t="str">
         <f t="shared" si="10"/>
@@ -3587,23 +3596,23 @@
         <v>92</v>
       </c>
       <c r="C17" s="75" t="s">
-        <v>137</v>
-      </c>
-      <c r="D17" s="113" t="s">
         <v>136</v>
+      </c>
+      <c r="D17" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="E17" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="F17" s="113" t="s">
-        <v>136</v>
+      <c r="F17" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="G17" s="75" t="str">
         <f t="shared" si="5"/>
         <v>twct_EOD_Tracer</v>
       </c>
       <c r="H17" s="75" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I17" s="74" t="s">
         <v>91</v>
@@ -3619,7 +3628,7 @@
         <v>75</v>
       </c>
       <c r="M17" s="74" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="N17" s="75" t="str">
         <f t="shared" ref="N17:N30" si="12">C17</f>
@@ -3641,26 +3650,26 @@
         <v>92</v>
       </c>
       <c r="C18" s="75" t="s">
-        <v>137</v>
-      </c>
-      <c r="D18" s="113" t="s">
         <v>136</v>
+      </c>
+      <c r="D18" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="E18" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="113" t="s">
-        <v>136</v>
+      <c r="F18" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="G18" s="75" t="str">
         <f t="shared" si="5"/>
         <v>twct_Number_of_Tracers</v>
       </c>
       <c r="H18" s="75" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I18" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J18" s="76" t="s">
         <v>124</v>
@@ -3671,7 +3680,7 @@
       </c>
       <c r="L18" s="77"/>
       <c r="M18" s="74" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="N18" s="75" t="str">
         <f t="shared" si="12"/>
@@ -3693,26 +3702,26 @@
         <v>92</v>
       </c>
       <c r="C19" s="75" t="s">
-        <v>137</v>
-      </c>
-      <c r="D19" s="113" t="s">
         <v>136</v>
+      </c>
+      <c r="D19" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="E19" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="F19" s="113" t="s">
-        <v>136</v>
+      <c r="F19" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="G19" s="75" t="str">
         <f t="shared" si="5"/>
         <v>twct_Frequency</v>
       </c>
       <c r="H19" s="75" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I19" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J19" s="76" t="s">
         <v>124</v>
@@ -3723,7 +3732,7 @@
       </c>
       <c r="L19" s="77"/>
       <c r="M19" s="74" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="N19" s="75" t="str">
         <f t="shared" si="12"/>
@@ -3745,26 +3754,26 @@
         <v>92</v>
       </c>
       <c r="C20" s="75" t="s">
-        <v>137</v>
-      </c>
-      <c r="D20" s="113" t="s">
         <v>136</v>
+      </c>
+      <c r="D20" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="E20" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="F20" s="113" t="s">
-        <v>136</v>
+      <c r="F20" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="G20" s="75" t="str">
         <f t="shared" si="5"/>
         <v>twct_Payment_Grace_Days</v>
       </c>
       <c r="H20" s="75" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I20" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J20" s="76" t="s">
         <v>124</v>
@@ -3775,7 +3784,7 @@
       </c>
       <c r="L20" s="77"/>
       <c r="M20" s="74" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="N20" s="75" t="str">
         <f t="shared" si="12"/>
@@ -3797,26 +3806,26 @@
         <v>92</v>
       </c>
       <c r="C21" s="75" t="s">
-        <v>137</v>
-      </c>
-      <c r="D21" s="113" t="s">
         <v>136</v>
+      </c>
+      <c r="D21" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="E21" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="113" t="s">
-        <v>136</v>
+      <c r="F21" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="G21" s="75" t="str">
         <f t="shared" si="5"/>
         <v>twct_Acceptance_Grace_days</v>
       </c>
       <c r="H21" s="75" t="s">
+        <v>133</v>
+      </c>
+      <c r="I21" s="74" t="s">
         <v>134</v>
-      </c>
-      <c r="I21" s="74" t="s">
-        <v>135</v>
       </c>
       <c r="J21" s="76" t="s">
         <v>124</v>
@@ -3827,7 +3836,7 @@
       </c>
       <c r="L21" s="77"/>
       <c r="M21" s="74" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="N21" s="75" t="str">
         <f t="shared" si="12"/>
@@ -3849,23 +3858,23 @@
         <v>92</v>
       </c>
       <c r="C22" s="106" t="s">
-        <v>138</v>
-      </c>
-      <c r="D22" s="113" t="s">
-        <v>136</v>
+        <v>137</v>
+      </c>
+      <c r="D22" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="E22" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="113" t="s">
-        <v>136</v>
+      <c r="F22" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="G22" s="75" t="str">
         <f t="shared" si="5"/>
         <v>twct_EOD_Tracer</v>
       </c>
       <c r="H22" s="75" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I22" s="74" t="s">
         <v>91</v>
@@ -3881,7 +3890,7 @@
         <v>75</v>
       </c>
       <c r="M22" s="74" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N22" s="75" t="str">
         <f t="shared" si="12"/>
@@ -3903,26 +3912,26 @@
         <v>92</v>
       </c>
       <c r="C23" s="106" t="s">
-        <v>138</v>
-      </c>
-      <c r="D23" s="113" t="s">
-        <v>136</v>
+        <v>137</v>
+      </c>
+      <c r="D23" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="E23" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="F23" s="113" t="s">
-        <v>136</v>
+      <c r="F23" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="G23" s="75" t="str">
         <f t="shared" si="5"/>
         <v>twct_Number_of_Tracers</v>
       </c>
       <c r="H23" s="75" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I23" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J23" s="76" t="s">
         <v>124</v>
@@ -3933,7 +3942,7 @@
       </c>
       <c r="L23" s="77"/>
       <c r="M23" s="74" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N23" s="75" t="str">
         <f t="shared" si="12"/>
@@ -3955,26 +3964,26 @@
         <v>92</v>
       </c>
       <c r="C24" s="106" t="s">
-        <v>138</v>
-      </c>
-      <c r="D24" s="113" t="s">
-        <v>136</v>
+        <v>137</v>
+      </c>
+      <c r="D24" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="E24" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="F24" s="113" t="s">
-        <v>136</v>
+      <c r="F24" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="G24" s="75" t="str">
         <f t="shared" si="5"/>
         <v>twct_Frequency</v>
       </c>
       <c r="H24" s="75" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I24" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J24" s="76" t="s">
         <v>124</v>
@@ -3985,7 +3994,7 @@
       </c>
       <c r="L24" s="77"/>
       <c r="M24" s="74" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N24" s="75" t="str">
         <f t="shared" si="12"/>
@@ -4007,26 +4016,26 @@
         <v>92</v>
       </c>
       <c r="C25" s="106" t="s">
-        <v>138</v>
-      </c>
-      <c r="D25" s="113" t="s">
-        <v>136</v>
+        <v>137</v>
+      </c>
+      <c r="D25" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="E25" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="F25" s="113" t="s">
-        <v>136</v>
+      <c r="F25" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="G25" s="75" t="str">
         <f t="shared" si="5"/>
         <v>twct_Payment_Grace_Days</v>
       </c>
       <c r="H25" s="75" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I25" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J25" s="76" t="s">
         <v>124</v>
@@ -4037,7 +4046,7 @@
       </c>
       <c r="L25" s="77"/>
       <c r="M25" s="74" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N25" s="75" t="str">
         <f t="shared" si="12"/>
@@ -4059,26 +4068,26 @@
         <v>92</v>
       </c>
       <c r="C26" s="106" t="s">
-        <v>138</v>
-      </c>
-      <c r="D26" s="113" t="s">
-        <v>136</v>
+        <v>137</v>
+      </c>
+      <c r="D26" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="E26" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="F26" s="113" t="s">
-        <v>136</v>
+      <c r="F26" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="G26" s="75" t="str">
         <f t="shared" si="5"/>
         <v>twct_Acceptance_Grace_days</v>
       </c>
       <c r="H26" s="75" t="s">
+        <v>133</v>
+      </c>
+      <c r="I26" s="74" t="s">
         <v>134</v>
-      </c>
-      <c r="I26" s="74" t="s">
-        <v>135</v>
       </c>
       <c r="J26" s="76" t="s">
         <v>124</v>
@@ -4089,7 +4098,7 @@
       </c>
       <c r="L26" s="77"/>
       <c r="M26" s="74" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N26" s="75" t="str">
         <f t="shared" si="12"/>
@@ -4111,23 +4120,23 @@
         <v>92</v>
       </c>
       <c r="C27" s="106" t="s">
-        <v>139</v>
-      </c>
-      <c r="D27" s="113" t="s">
-        <v>136</v>
+        <v>138</v>
+      </c>
+      <c r="D27" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="E27" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="F27" s="113" t="s">
-        <v>136</v>
+      <c r="F27" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="G27" s="75" t="str">
         <f t="shared" si="5"/>
         <v>twct_EOD_Tracer</v>
       </c>
       <c r="H27" s="75" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I27" s="74" t="s">
         <v>91</v>
@@ -4143,7 +4152,7 @@
         <v>75</v>
       </c>
       <c r="M27" s="74" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N27" s="75" t="str">
         <f t="shared" si="12"/>
@@ -4165,26 +4174,26 @@
         <v>92</v>
       </c>
       <c r="C28" s="106" t="s">
-        <v>139</v>
-      </c>
-      <c r="D28" s="113" t="s">
-        <v>136</v>
+        <v>138</v>
+      </c>
+      <c r="D28" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="E28" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="F28" s="113" t="s">
-        <v>136</v>
+      <c r="F28" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="G28" s="75" t="str">
         <f t="shared" si="5"/>
         <v>twct_Number_of_Tracers</v>
       </c>
       <c r="H28" s="75" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I28" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J28" s="76" t="s">
         <v>124</v>
@@ -4195,7 +4204,7 @@
       </c>
       <c r="L28" s="77"/>
       <c r="M28" s="74" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N28" s="75" t="str">
         <f t="shared" si="12"/>
@@ -4217,26 +4226,26 @@
         <v>92</v>
       </c>
       <c r="C29" s="106" t="s">
-        <v>139</v>
-      </c>
-      <c r="D29" s="113" t="s">
-        <v>136</v>
+        <v>138</v>
+      </c>
+      <c r="D29" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="E29" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="F29" s="113" t="s">
-        <v>136</v>
+      <c r="F29" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="G29" s="75" t="str">
         <f t="shared" si="5"/>
         <v>twct_Frequency</v>
       </c>
       <c r="H29" s="75" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I29" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J29" s="76" t="s">
         <v>124</v>
@@ -4247,7 +4256,7 @@
       </c>
       <c r="L29" s="77"/>
       <c r="M29" s="74" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N29" s="75" t="str">
         <f t="shared" si="12"/>
@@ -4269,26 +4278,26 @@
         <v>92</v>
       </c>
       <c r="C30" s="106" t="s">
-        <v>139</v>
-      </c>
-      <c r="D30" s="113" t="s">
-        <v>136</v>
+        <v>138</v>
+      </c>
+      <c r="D30" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="E30" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="F30" s="113" t="s">
-        <v>136</v>
+      <c r="F30" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="G30" s="75" t="str">
         <f t="shared" si="5"/>
         <v>twct_Payment_Grace_Days</v>
       </c>
       <c r="H30" s="75" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I30" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J30" s="76" t="s">
         <v>124</v>
@@ -4299,7 +4308,7 @@
       </c>
       <c r="L30" s="77"/>
       <c r="M30" s="74" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N30" s="75" t="str">
         <f t="shared" si="12"/>
@@ -4321,26 +4330,26 @@
         <v>92</v>
       </c>
       <c r="C31" s="106" t="s">
-        <v>139</v>
-      </c>
-      <c r="D31" s="113" t="s">
-        <v>136</v>
+        <v>138</v>
+      </c>
+      <c r="D31" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="E31" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="F31" s="113" t="s">
-        <v>136</v>
+      <c r="F31" s="107" t="s">
+        <v>135</v>
       </c>
       <c r="G31" s="75" t="str">
         <f t="shared" si="5"/>
         <v>twct_Acceptance_Grace_days</v>
       </c>
       <c r="H31" s="75" t="s">
+        <v>133</v>
+      </c>
+      <c r="I31" s="74" t="s">
         <v>134</v>
-      </c>
-      <c r="I31" s="74" t="s">
-        <v>135</v>
       </c>
       <c r="J31" s="76" t="s">
         <v>124</v>
@@ -4351,7 +4360,7 @@
       </c>
       <c r="L31" s="77"/>
       <c r="M31" s="74" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N31" s="75" t="str">
         <f t="shared" ref="N31" si="14">C31</f>
@@ -6699,105 +6708,105 @@
       <c r="N260" s="91"/>
       <c r="O260" s="91"/>
     </row>
-    <row r="262" spans="3:15" ht="15.75">
+    <row r="262" spans="3:15">
       <c r="G262" s="92"/>
       <c r="H262" s="92"/>
       <c r="I262" s="92"/>
       <c r="J262" s="78"/>
       <c r="M262" s="91"/>
     </row>
-    <row r="263" spans="3:15" ht="15.75">
+    <row r="263" spans="3:15">
       <c r="G263" s="92"/>
       <c r="H263" s="92"/>
       <c r="I263" s="92"/>
       <c r="J263" s="78"/>
       <c r="M263" s="91"/>
     </row>
-    <row r="264" spans="3:15" ht="15.75">
+    <row r="264" spans="3:15">
       <c r="G264" s="92"/>
       <c r="H264" s="92"/>
       <c r="I264" s="92"/>
       <c r="J264" s="78"/>
       <c r="M264" s="91"/>
     </row>
-    <row r="265" spans="3:15" ht="15.75">
+    <row r="265" spans="3:15">
       <c r="G265" s="92"/>
       <c r="H265" s="92"/>
       <c r="I265" s="92"/>
       <c r="J265" s="78"/>
       <c r="M265" s="91"/>
     </row>
-    <row r="266" spans="3:15" ht="15.75">
+    <row r="266" spans="3:15">
       <c r="G266" s="92"/>
       <c r="H266" s="92"/>
       <c r="I266" s="92"/>
       <c r="J266" s="78"/>
       <c r="M266" s="91"/>
     </row>
-    <row r="268" spans="3:15" ht="15.75">
+    <row r="268" spans="3:15">
       <c r="G268" s="92"/>
       <c r="H268" s="92"/>
       <c r="I268" s="92"/>
       <c r="J268" s="78"/>
       <c r="M268" s="91"/>
     </row>
-    <row r="269" spans="3:15" ht="15.75">
+    <row r="269" spans="3:15">
       <c r="G269" s="92"/>
       <c r="H269" s="92"/>
       <c r="I269" s="92"/>
       <c r="J269" s="78"/>
       <c r="M269" s="91"/>
     </row>
-    <row r="270" spans="3:15" ht="15.75">
+    <row r="270" spans="3:15">
       <c r="G270" s="92"/>
       <c r="H270" s="92"/>
       <c r="I270" s="92"/>
       <c r="J270" s="78"/>
       <c r="M270" s="91"/>
     </row>
-    <row r="271" spans="3:15" ht="15.75">
+    <row r="271" spans="3:15">
       <c r="G271" s="92"/>
       <c r="H271" s="92"/>
       <c r="I271" s="92"/>
       <c r="J271" s="78"/>
       <c r="M271" s="91"/>
     </row>
-    <row r="272" spans="3:15" ht="15.75">
+    <row r="272" spans="3:15">
       <c r="G272" s="92"/>
       <c r="H272" s="92"/>
       <c r="I272" s="92"/>
       <c r="J272" s="78"/>
       <c r="M272" s="91"/>
     </row>
-    <row r="274" spans="7:13" ht="15.75">
+    <row r="274" spans="7:13">
       <c r="G274" s="92"/>
       <c r="H274" s="92"/>
       <c r="I274" s="92"/>
       <c r="J274" s="78"/>
       <c r="M274" s="91"/>
     </row>
-    <row r="275" spans="7:13" ht="15.75">
+    <row r="275" spans="7:13">
       <c r="G275" s="92"/>
       <c r="H275" s="92"/>
       <c r="I275" s="92"/>
       <c r="J275" s="78"/>
       <c r="M275" s="91"/>
     </row>
-    <row r="276" spans="7:13" ht="15.75">
+    <row r="276" spans="7:13">
       <c r="G276" s="92"/>
       <c r="H276" s="92"/>
       <c r="I276" s="92"/>
       <c r="J276" s="78"/>
       <c r="M276" s="91"/>
     </row>
-    <row r="277" spans="7:13" ht="15.75">
+    <row r="277" spans="7:13">
       <c r="G277" s="92"/>
       <c r="H277" s="92"/>
       <c r="I277" s="92"/>
       <c r="J277" s="78"/>
       <c r="M277" s="91"/>
     </row>
-    <row r="278" spans="7:13" ht="15.75">
+    <row r="278" spans="7:13">
       <c r="G278" s="92"/>
       <c r="H278" s="92"/>
       <c r="I278" s="92"/>
@@ -6819,7 +6828,7 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="33.85546875" style="59" customWidth="1"/>
     <col min="3" max="3" width="32.85546875" style="59" customWidth="1"/>
@@ -7256,91 +7265,91 @@
       <c r="C53" s="69"/>
       <c r="D53" s="56"/>
     </row>
-    <row r="54" spans="1:4" ht="15.75" thickBot="1">
+    <row r="54" spans="1:4" ht="16.5" thickBot="1">
       <c r="A54" s="68"/>
       <c r="B54" s="68"/>
       <c r="C54" s="69"/>
       <c r="D54" s="70"/>
     </row>
-    <row r="55" spans="1:4" ht="15.75" thickBot="1">
+    <row r="55" spans="1:4" ht="16.5" thickBot="1">
       <c r="A55" s="50"/>
       <c r="B55" s="51"/>
       <c r="C55" s="51"/>
       <c r="D55" s="52"/>
     </row>
-    <row r="56" spans="1:4" ht="15.75" thickBot="1">
+    <row r="56" spans="1:4" ht="16.5" thickBot="1">
       <c r="A56" s="53"/>
       <c r="B56" s="54"/>
       <c r="C56" s="54"/>
       <c r="D56" s="55"/>
     </row>
-    <row r="57" spans="1:4" ht="15.75" thickBot="1">
+    <row r="57" spans="1:4" ht="16.5" thickBot="1">
       <c r="A57" s="53"/>
       <c r="B57" s="54"/>
       <c r="C57" s="54"/>
       <c r="D57" s="55"/>
     </row>
-    <row r="58" spans="1:4" ht="15.75" thickBot="1">
+    <row r="58" spans="1:4" ht="16.5" thickBot="1">
       <c r="A58" s="56"/>
       <c r="B58" s="56"/>
       <c r="C58" s="51"/>
       <c r="D58" s="70"/>
     </row>
-    <row r="59" spans="1:4" ht="15.75" thickBot="1">
+    <row r="59" spans="1:4" ht="16.5" thickBot="1">
       <c r="A59" s="68"/>
       <c r="B59" s="102"/>
       <c r="C59" s="54"/>
       <c r="D59" s="70"/>
     </row>
-    <row r="60" spans="1:4" ht="15.75" thickBot="1">
+    <row r="60" spans="1:4" ht="16.5" thickBot="1">
       <c r="A60" s="68"/>
       <c r="B60" s="102"/>
       <c r="C60" s="54"/>
       <c r="D60" s="70"/>
     </row>
-    <row r="61" spans="1:4" ht="15.75">
-      <c r="A61" s="107"/>
+    <row r="61" spans="1:4">
+      <c r="A61" s="108"/>
       <c r="B61" s="98"/>
-      <c r="C61" s="109"/>
-      <c r="D61" s="109"/>
+      <c r="C61" s="110"/>
+      <c r="D61" s="110"/>
     </row>
     <row r="62" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A62" s="108"/>
+      <c r="A62" s="109"/>
       <c r="B62" s="99"/>
-      <c r="C62" s="110"/>
-      <c r="D62" s="110"/>
-    </row>
-    <row r="63" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C62" s="111"/>
+      <c r="D62" s="111"/>
+    </row>
+    <row r="63" spans="1:4" ht="16.5" thickBot="1">
       <c r="A63" s="93"/>
       <c r="B63" s="94"/>
       <c r="C63" s="94"/>
       <c r="D63" s="94"/>
     </row>
-    <row r="64" spans="1:4" ht="15.75" thickBot="1">
+    <row r="64" spans="1:4" ht="16.5" thickBot="1">
       <c r="A64" s="93"/>
       <c r="B64" s="94"/>
       <c r="C64" s="94"/>
       <c r="D64" s="95"/>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="111"/>
+      <c r="A65" s="112"/>
       <c r="B65" s="100"/>
-      <c r="C65" s="111"/>
-      <c r="D65" s="111"/>
-    </row>
-    <row r="66" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A66" s="112"/>
+      <c r="C65" s="112"/>
+      <c r="D65" s="112"/>
+    </row>
+    <row r="66" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A66" s="113"/>
       <c r="B66" s="101"/>
-      <c r="C66" s="112"/>
-      <c r="D66" s="112"/>
-    </row>
-    <row r="67" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C66" s="113"/>
+      <c r="D66" s="113"/>
+    </row>
+    <row r="67" spans="1:4" ht="16.5" thickBot="1">
       <c r="A67" s="96"/>
       <c r="B67" s="96"/>
       <c r="C67" s="96"/>
       <c r="D67" s="96"/>
     </row>
-    <row r="68" spans="1:4" ht="15.75" thickBot="1">
+    <row r="68" spans="1:4" ht="16.5" thickBot="1">
       <c r="A68" s="96"/>
       <c r="B68" s="96"/>
       <c r="C68" s="96"/>
@@ -7355,6 +7364,7 @@
     <mergeCell ref="C65:C66"/>
     <mergeCell ref="D65:D66"/>
   </mergeCells>
+  <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7367,7 +7377,7 @@
       <selection activeCell="B1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
@@ -7376,6 +7386,7 @@
     <col min="5" max="5" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData/>
+  <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>